<commit_message>
first kinda working algo
</commit_message>
<xml_diff>
--- a/Data/last_week_prices.xlsx
+++ b/Data/last_week_prices.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\hakaton 2\upravtok\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8F8A80E3-5CEE-4FDA-A458-EBD40BCF0080}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF0CC6A5-97C2-405C-B029-32347E3E06A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CC4CAC88-C493-410A-AC04-375936CAED5A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="33">
   <si>
     <t>Sat, 03/09</t>
   </si>
@@ -99,16 +99,58 @@
   </si>
   <si>
     <t>23 - 24</t>
+  </si>
+  <si>
+    <t>1 - 2</t>
+  </si>
+  <si>
+    <t>3 - 4</t>
+  </si>
+  <si>
+    <t>4 - 5</t>
+  </si>
+  <si>
+    <t>2 - 3</t>
+  </si>
+  <si>
+    <t>6 - 7</t>
+  </si>
+  <si>
+    <t>7 - 8</t>
+  </si>
+  <si>
+    <t>9 - 10</t>
+  </si>
+  <si>
+    <t>11 - 12</t>
+  </si>
+  <si>
+    <t>12 - 13</t>
+  </si>
+  <si>
+    <t>5 - 6</t>
+  </si>
+  <si>
+    <t>8 - 9</t>
+  </si>
+  <si>
+    <t>10 - 11</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -136,7 +178,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -474,10 +516,13 @@
   <dimension ref="A1:I49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="53.140625" style="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
@@ -503,7 +548,7 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B2" t="s">
@@ -558,8 +603,8 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>45293</v>
+      <c r="A4" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
@@ -613,8 +658,8 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>45325</v>
+      <c r="A6" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
@@ -668,8 +713,8 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>45355</v>
+      <c r="A8" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
@@ -723,8 +768,8 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>45387</v>
+      <c r="A10" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="B10" t="s">
         <v>8</v>
@@ -778,8 +823,8 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>45418</v>
+      <c r="A12" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="B12" t="s">
         <v>8</v>
@@ -833,8 +878,8 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>45450</v>
+      <c r="A14" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="B14" t="s">
         <v>8</v>
@@ -888,8 +933,8 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>45481</v>
+      <c r="A16" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="B16" t="s">
         <v>8</v>
@@ -943,8 +988,8 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <v>45513</v>
+      <c r="A18" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="B18" t="s">
         <v>8</v>
@@ -998,8 +1043,8 @@
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <v>45545</v>
+      <c r="A20" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="B20" t="s">
         <v>8</v>
@@ -1053,8 +1098,8 @@
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
-        <v>45576</v>
+      <c r="A22" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="B22" t="s">
         <v>8</v>
@@ -1108,8 +1153,8 @@
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
-        <v>45608</v>
+      <c r="A24" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="B24" t="s">
         <v>8</v>
@@ -1163,8 +1208,8 @@
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
-        <v>45639</v>
+      <c r="A26" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="B26" t="s">
         <v>8</v>
@@ -1218,7 +1263,7 @@
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="A28" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B28" t="s">
@@ -1273,7 +1318,7 @@
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="A30" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B30" t="s">
@@ -1328,7 +1373,7 @@
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="A32" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B32" t="s">
@@ -1383,7 +1428,7 @@
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="A34" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B34" t="s">
@@ -1438,7 +1483,7 @@
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="A36" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B36" t="s">
@@ -1493,7 +1538,7 @@
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="A38" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B38" t="s">
@@ -1548,7 +1593,7 @@
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="A40" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B40" t="s">
@@ -1603,7 +1648,7 @@
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="A42" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B42" t="s">
@@ -1658,7 +1703,7 @@
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+      <c r="A44" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B44" t="s">
@@ -1713,7 +1758,7 @@
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+      <c r="A46" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B46" t="s">
@@ -1768,7 +1813,7 @@
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+      <c r="A48" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B48" t="s">
@@ -1823,6 +1868,8 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>